<commit_message>
Added Fish Pop Table to excel Calc
</commit_message>
<xml_diff>
--- a/Excel_Calc/Simple Calculator.xlsx
+++ b/Excel_Calc/Simple Calculator.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwilkinson/Documents/GitHub/FEWnopoly/Excel_Calc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sammy\Documents\GitHub\FEWnopoly\Excel_Calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF3290E-9278-1445-8BB4-B884E0680D51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E48BF06-5920-4860-9A40-B28E278F13B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
   <si>
     <t>Color Key</t>
   </si>
@@ -170,13 +178,55 @@
   </si>
   <si>
     <t>Initial Setup</t>
+  </si>
+  <si>
+    <t>Fish population</t>
+  </si>
+  <si>
+    <t>49-45</t>
+  </si>
+  <si>
+    <t>44-40</t>
+  </si>
+  <si>
+    <t>39-35</t>
+  </si>
+  <si>
+    <t>34-30</t>
+  </si>
+  <si>
+    <t>29-25</t>
+  </si>
+  <si>
+    <t>24-20</t>
+  </si>
+  <si>
+    <t>19-15</t>
+  </si>
+  <si>
+    <t>14-10</t>
+  </si>
+  <si>
+    <t>Surface water level</t>
+  </si>
+  <si>
+    <t>20+</t>
+  </si>
+  <si>
+    <t>19-16</t>
+  </si>
+  <si>
+    <t>15-12</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -191,8 +241,27 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,8 +310,26 @@
         <bgColor rgb="FF00CECE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEF2CB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD6EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -364,11 +451,145 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -405,6 +626,48 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,26 +987,26 @@
   </sheetPr>
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
+    <sheetView zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" customWidth="1"/>
-    <col min="5" max="5" width="22.5" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -751,33 +1014,33 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>49</v>
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
@@ -805,7 +1068,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>11</v>
       </c>
@@ -833,7 +1096,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
       <c r="D10" s="17" t="s">
@@ -856,12 +1119,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
@@ -872,7 +1135,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
@@ -895,7 +1158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
@@ -904,12 +1167,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
@@ -929,7 +1192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="24" t="s">
         <v>30</v>
       </c>
@@ -942,7 +1205,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>33</v>
       </c>
@@ -951,12 +1214,12 @@
         <v>7.666666666666667</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>35</v>
       </c>
@@ -964,7 +1227,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>37</v>
       </c>
@@ -975,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>39</v>
       </c>
@@ -986,7 +1249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>40</v>
       </c>
@@ -997,7 +1260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>41</v>
       </c>
@@ -1008,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
         <v>42</v>
       </c>
@@ -1017,7 +1280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>43</v>
       </c>
@@ -1031,7 +1294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>45</v>
       </c>
@@ -1047,12 +1310,12 @@
         <v>26.333333333333332</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>35</v>
       </c>
@@ -1060,7 +1323,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>37</v>
       </c>
@@ -1071,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>39</v>
       </c>
@@ -1082,7 +1345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>40</v>
       </c>
@@ -1093,7 +1356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>41</v>
       </c>
@@ -1104,7 +1367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="3" t="s">
         <v>42</v>
       </c>
@@ -1113,7 +1376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
         <v>43</v>
       </c>
@@ -1127,7 +1390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
         <v>45</v>
       </c>
@@ -1143,16 +1406,16 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="27"/>
       <c r="E42" s="27"/>
     </row>
-    <row r="43" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>35</v>
       </c>
@@ -1160,7 +1423,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>37</v>
       </c>
@@ -1171,7 +1434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>39</v>
       </c>
@@ -1182,7 +1445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>40</v>
       </c>
@@ -1193,7 +1456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>41</v>
       </c>
@@ -1204,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C49" s="3" t="s">
         <v>42</v>
       </c>
@@ -1213,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>43</v>
       </c>
@@ -1227,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>45</v>
       </c>
@@ -1243,10 +1506,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="2:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D52" s="27"/>
     </row>
-    <row r="54" spans="2:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C54" s="27"/>
       <c r="E54" s="27"/>
     </row>
@@ -1271,7 +1534,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41 C31 C51">
+  <conditionalFormatting sqref="C31 C41 C51">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="formula" val="E9"/>
@@ -1301,7 +1564,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C51 C41">
+  <conditionalFormatting sqref="C41 C51">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="E9"/>
@@ -1333,4 +1596,292 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF29A73-2493-4C59-A4AD-4E670054F4FB}">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="38"/>
+    </row>
+    <row r="2" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="33">
+        <v>43713</v>
+      </c>
+      <c r="L2" s="33">
+        <v>43556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="31">
+        <v>5</v>
+      </c>
+      <c r="D3" s="31">
+        <v>5</v>
+      </c>
+      <c r="E3" s="31">
+        <v>5</v>
+      </c>
+      <c r="F3" s="31">
+        <v>4</v>
+      </c>
+      <c r="G3" s="31">
+        <v>4</v>
+      </c>
+      <c r="H3" s="31">
+        <v>3</v>
+      </c>
+      <c r="I3" s="31">
+        <v>2</v>
+      </c>
+      <c r="J3" s="31">
+        <v>2</v>
+      </c>
+      <c r="K3" s="31">
+        <v>1</v>
+      </c>
+      <c r="L3" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="40"/>
+      <c r="B4" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="31">
+        <v>3</v>
+      </c>
+      <c r="D4" s="31">
+        <v>2</v>
+      </c>
+      <c r="E4" s="31">
+        <v>2</v>
+      </c>
+      <c r="F4" s="31">
+        <v>2</v>
+      </c>
+      <c r="G4" s="31">
+        <v>1</v>
+      </c>
+      <c r="H4" s="31">
+        <v>1</v>
+      </c>
+      <c r="I4" s="31">
+        <v>0</v>
+      </c>
+      <c r="J4" s="31">
+        <v>0</v>
+      </c>
+      <c r="K4" s="31">
+        <v>0</v>
+      </c>
+      <c r="L4" s="31">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="40"/>
+      <c r="B5" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="31">
+        <v>-6</v>
+      </c>
+      <c r="D5" s="31">
+        <v>-6</v>
+      </c>
+      <c r="E5" s="31">
+        <v>-6</v>
+      </c>
+      <c r="F5" s="31">
+        <v>-5</v>
+      </c>
+      <c r="G5" s="31">
+        <v>-5</v>
+      </c>
+      <c r="H5" s="31">
+        <v>-4</v>
+      </c>
+      <c r="I5" s="31">
+        <v>-3</v>
+      </c>
+      <c r="J5" s="31">
+        <v>-3</v>
+      </c>
+      <c r="K5" s="31">
+        <v>-3</v>
+      </c>
+      <c r="L5" s="31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="40"/>
+      <c r="B6" s="35">
+        <v>43777</v>
+      </c>
+      <c r="C6" s="31">
+        <v>-12</v>
+      </c>
+      <c r="D6" s="31">
+        <v>-10</v>
+      </c>
+      <c r="E6" s="31">
+        <v>-8</v>
+      </c>
+      <c r="F6" s="31">
+        <v>-7</v>
+      </c>
+      <c r="G6" s="31">
+        <v>-6</v>
+      </c>
+      <c r="H6" s="31">
+        <v>-6</v>
+      </c>
+      <c r="I6" s="31">
+        <v>-6</v>
+      </c>
+      <c r="J6" s="31">
+        <v>-6</v>
+      </c>
+      <c r="K6" s="31">
+        <v>-6</v>
+      </c>
+      <c r="L6" s="31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="40"/>
+      <c r="B7" s="35">
+        <v>43650</v>
+      </c>
+      <c r="C7" s="31">
+        <v>-20</v>
+      </c>
+      <c r="D7" s="31">
+        <v>-16</v>
+      </c>
+      <c r="E7" s="31">
+        <v>-14</v>
+      </c>
+      <c r="F7" s="31">
+        <v>-12</v>
+      </c>
+      <c r="G7" s="31">
+        <v>-10</v>
+      </c>
+      <c r="H7" s="31">
+        <v>-9</v>
+      </c>
+      <c r="I7" s="31">
+        <v>-9</v>
+      </c>
+      <c r="J7" s="31">
+        <v>-8</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="L7" s="31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="41"/>
+      <c r="B8" s="35">
+        <v>43525</v>
+      </c>
+      <c r="C8" s="31">
+        <v>-44</v>
+      </c>
+      <c r="D8" s="31">
+        <v>-39</v>
+      </c>
+      <c r="E8" s="31">
+        <v>-34</v>
+      </c>
+      <c r="F8" s="31">
+        <v>-29</v>
+      </c>
+      <c r="G8" s="31">
+        <v>-24</v>
+      </c>
+      <c r="H8" s="31">
+        <v>-19</v>
+      </c>
+      <c r="I8" s="31">
+        <v>-14</v>
+      </c>
+      <c r="J8" s="31">
+        <v>-9</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="L8" s="31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="A3:A8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated fish pop table
</commit_message>
<xml_diff>
--- a/Excel_Calc/Simple Calculator.xlsx
+++ b/Excel_Calc/Simple Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sammy\Documents\GitHub\FEWnopoly\Excel_Calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E48BF06-5920-4860-9A40-B28E278F13B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3392E31-E7EC-4D20-B0FB-2E4665B40C9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="69">
   <si>
     <t>Color Key</t>
   </si>
@@ -220,6 +220,21 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>9-5</t>
+  </si>
+  <si>
+    <t>4-1</t>
+  </si>
+  <si>
+    <t>11-8</t>
+  </si>
+  <si>
+    <t>7-5</t>
+  </si>
+  <si>
+    <t>3-1</t>
   </si>
 </sst>
 </file>
@@ -236,10 +251,12 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -641,13 +658,7 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -666,6 +677,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1534,7 +1551,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31 C41 C51">
+  <conditionalFormatting sqref="C41 C31 C51">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="formula" val="E9"/>
@@ -1564,7 +1581,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41 C51">
+  <conditionalFormatting sqref="C51 C41">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="E9"/>
@@ -1603,26 +1620,26 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="38"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="36"/>
     </row>
     <row r="2" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="30"/>
@@ -1651,18 +1668,18 @@
       <c r="J2" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="33">
-        <v>43713</v>
-      </c>
-      <c r="L2" s="33">
-        <v>43556</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="K2" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="33" t="s">
         <v>60</v>
       </c>
       <c r="C3" s="31">
@@ -1697,8 +1714,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
-      <c r="B4" s="34" t="s">
+      <c r="A4" s="38"/>
+      <c r="B4" s="33" t="s">
         <v>61</v>
       </c>
       <c r="C4" s="31">
@@ -1733,8 +1750,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
-      <c r="B5" s="34" t="s">
+      <c r="A5" s="38"/>
+      <c r="B5" s="33" t="s">
         <v>62</v>
       </c>
       <c r="C5" s="31">
@@ -1769,9 +1786,9 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
-      <c r="B6" s="35">
-        <v>43777</v>
+      <c r="A6" s="38"/>
+      <c r="B6" s="41" t="s">
+        <v>66</v>
       </c>
       <c r="C6" s="31">
         <v>-12</v>
@@ -1805,9 +1822,9 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
-      <c r="B7" s="35">
-        <v>43650</v>
+      <c r="A7" s="38"/>
+      <c r="B7" s="41" t="s">
+        <v>67</v>
       </c>
       <c r="C7" s="31">
         <v>-20</v>
@@ -1841,9 +1858,9 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="41"/>
-      <c r="B8" s="35">
-        <v>43525</v>
+      <c r="A8" s="39"/>
+      <c r="B8" s="41" t="s">
+        <v>68</v>
       </c>
       <c r="C8" s="31">
         <v>-44</v>

</xml_diff>